<commit_message>
feat(tests): added C as well as B reflector to  test
</commit_message>
<xml_diff>
--- a/rotor-ring-map-remapped.xlsx
+++ b/rotor-ring-map-remapped.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pat.hearps/Documents/DataScienceStudy/ENIGMA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE2D33E-194F-0B45-89F4-51A48B9816A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A59F6E-F905-1A44-8857-BE0833FC35FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="460" windowWidth="28040" windowHeight="16380" xr2:uid="{A35B3064-C88D-FE40-A178-BB01BEFC4815}"/>
   </bookViews>
@@ -1043,7 +1043,7 @@
   <dimension ref="A1:AW77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1214,6 +1214,10 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
+      <c r="T4" s="2" t="str">
+        <f>_xlfn.CONCAT(U11:U36)</f>
+        <v>YRUHQSLDPXNGOKMIEBFZCWVJAT</v>
+      </c>
       <c r="U4" s="1"/>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
@@ -1329,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="U6" s="47" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD6" s="11" t="s">
         <v>33</v>
@@ -1878,7 +1882,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>0</v>
       </c>
@@ -1943,8 +1947,9 @@
       <c r="T11" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="U11" s="18" t="s">
-        <v>24</v>
+      <c r="U11" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T11,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>Y</v>
       </c>
       <c r="V11" s="25" t="s">
         <v>0</v>
@@ -2111,8 +2116,9 @@
       <c r="T12" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="U12" s="17" t="s">
-        <v>17</v>
+      <c r="U12" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T12,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>R</v>
       </c>
       <c r="V12" s="25" t="s">
         <v>1</v>
@@ -2279,8 +2285,9 @@
       <c r="T13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="U13" s="17" t="s">
-        <v>20</v>
+      <c r="U13" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T13,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>U</v>
       </c>
       <c r="V13" s="25" t="s">
         <v>2</v>
@@ -2447,8 +2454,9 @@
       <c r="T14" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U14" s="17" t="s">
-        <v>7</v>
+      <c r="U14" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T14,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>H</v>
       </c>
       <c r="V14" s="25" t="s">
         <v>3</v>
@@ -2615,8 +2623,9 @@
       <c r="T15" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="U15" s="17" t="s">
-        <v>16</v>
+      <c r="U15" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T15,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>Q</v>
       </c>
       <c r="V15" s="25" t="s">
         <v>4</v>
@@ -2783,8 +2792,9 @@
       <c r="T16" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="U16" s="17" t="s">
-        <v>18</v>
+      <c r="U16" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T16,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>S</v>
       </c>
       <c r="V16" s="25" t="s">
         <v>5</v>
@@ -2951,8 +2961,9 @@
       <c r="T17" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="U17" s="17" t="s">
-        <v>11</v>
+      <c r="U17" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T17,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>L</v>
       </c>
       <c r="V17" s="25" t="s">
         <v>6</v>
@@ -3119,8 +3130,9 @@
       <c r="T18" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="U18" s="17" t="s">
-        <v>3</v>
+      <c r="U18" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T18,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>D</v>
       </c>
       <c r="V18" s="25" t="s">
         <v>7</v>
@@ -3287,8 +3299,9 @@
       <c r="T19" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="U19" s="17" t="s">
-        <v>15</v>
+      <c r="U19" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T19,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>P</v>
       </c>
       <c r="V19" s="25" t="s">
         <v>8</v>
@@ -3455,8 +3468,9 @@
       <c r="T20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="U20" s="17" t="s">
-        <v>23</v>
+      <c r="U20" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T20,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>X</v>
       </c>
       <c r="V20" s="25" t="s">
         <v>9</v>
@@ -3623,8 +3637,9 @@
       <c r="T21" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="U21" s="17" t="s">
-        <v>13</v>
+      <c r="U21" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T21,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>N</v>
       </c>
       <c r="V21" s="25" t="s">
         <v>10</v>
@@ -3791,8 +3806,9 @@
       <c r="T22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="U22" s="17" t="s">
-        <v>6</v>
+      <c r="U22" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T22,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>G</v>
       </c>
       <c r="V22" s="25" t="s">
         <v>11</v>
@@ -3959,8 +3975,9 @@
       <c r="T23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="U23" s="17" t="s">
-        <v>14</v>
+      <c r="U23" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T23,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>O</v>
       </c>
       <c r="V23" s="25" t="s">
         <v>12</v>
@@ -4127,8 +4144,9 @@
       <c r="T24" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="U24" s="17" t="s">
-        <v>10</v>
+      <c r="U24" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T24,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>K</v>
       </c>
       <c r="V24" s="25" t="s">
         <v>13</v>
@@ -4295,8 +4313,9 @@
       <c r="T25" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="U25" s="17" t="s">
-        <v>12</v>
+      <c r="U25" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T25,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>M</v>
       </c>
       <c r="V25" s="25" t="s">
         <v>14</v>
@@ -4463,8 +4482,9 @@
       <c r="T26" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="U26" s="17" t="s">
-        <v>8</v>
+      <c r="U26" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T26,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>I</v>
       </c>
       <c r="V26" s="25" t="s">
         <v>15</v>
@@ -4631,8 +4651,9 @@
       <c r="T27" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="U27" s="17" t="s">
-        <v>4</v>
+      <c r="U27" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T27,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>E</v>
       </c>
       <c r="V27" s="25" t="s">
         <v>16</v>
@@ -4799,8 +4820,9 @@
       <c r="T28" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="U28" s="17" t="s">
-        <v>1</v>
+      <c r="U28" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T28,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>B</v>
       </c>
       <c r="V28" s="25" t="s">
         <v>17</v>
@@ -4967,8 +4989,9 @@
       <c r="T29" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="U29" s="17" t="s">
-        <v>5</v>
+      <c r="U29" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T29,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>F</v>
       </c>
       <c r="V29" s="25" t="s">
         <v>18</v>
@@ -5135,8 +5158,9 @@
       <c r="T30" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="U30" s="17" t="s">
-        <v>25</v>
+      <c r="U30" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T30,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>Z</v>
       </c>
       <c r="V30" s="25" t="s">
         <v>19</v>
@@ -5303,8 +5327,9 @@
       <c r="T31" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="U31" s="17" t="s">
-        <v>2</v>
+      <c r="U31" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T31,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>C</v>
       </c>
       <c r="V31" s="25" t="s">
         <v>20</v>
@@ -5471,8 +5496,9 @@
       <c r="T32" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="U32" s="17" t="s">
-        <v>22</v>
+      <c r="U32" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T32,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>W</v>
       </c>
       <c r="V32" s="25" t="s">
         <v>21</v>
@@ -5639,8 +5665,9 @@
       <c r="T33" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="U33" s="17" t="s">
-        <v>21</v>
+      <c r="U33" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T33,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>V</v>
       </c>
       <c r="V33" s="25" t="s">
         <v>22</v>
@@ -5807,8 +5834,9 @@
       <c r="T34" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="U34" s="17" t="s">
-        <v>9</v>
+      <c r="U34" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T34,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>J</v>
       </c>
       <c r="V34" s="25" t="s">
         <v>23</v>
@@ -5975,8 +6003,9 @@
       <c r="T35" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="U35" s="17" t="s">
-        <v>0</v>
+      <c r="U35" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T35,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>A</v>
       </c>
       <c r="V35" s="25" t="s">
         <v>24</v>
@@ -6143,8 +6172,9 @@
       <c r="T36" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="U36" s="17" t="s">
-        <v>19</v>
+      <c r="U36" s="16" t="str">
+        <f>INDEX(rotors!$B$32:$C$57,MATCH(T36,rotors!$A$32:$A$57),MATCH(U$9,rotors!$B$31:$C$31,0))</f>
+        <v>T</v>
       </c>
       <c r="V36" s="25" t="s">
         <v>25</v>
@@ -7135,8 +7165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF50C79-16D5-6949-8056-A6FABF62AFFF}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7547,205 +7577,283 @@
       <c r="B32" s="18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B35" s="17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B42" s="17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B53" s="17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>19</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>